<commit_message>
updated command line execution of network analysis
</commit_message>
<xml_diff>
--- a/Data/Database_Citations.xlsx
+++ b/Data/Database_Citations.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkhuang/Documents/Ideker_Lab/Network_Evaluation_Tools/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\users\jkhuang\Data\Projects\Network_Analysis\Network_Evaluation_Tools\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16875" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="131">
   <si>
     <t>Network Name</t>
   </si>
@@ -417,12 +417,15 @@
   </si>
   <si>
     <t>Snel B, Lehmann G, Bork P, Huynen MA. STRING: a web-server to retrieve and display the repeatedly occurring neighbourhood of a gene. Nucleic Acids Res. 2000 Sep 15;28(18):3442-4.</t>
+  </si>
+  <si>
+    <t>Szklarcyk D, Morris JH, Cook H, Kuhn M, Wyder S, Simonovic M, Santos A, Doncheva NT, Rother A, Bork P, Jensen L, von Mering C. The STRING database in 2017: quality-controlled protein–protein association networks, made broadly accessible. Nucleic Acids Res. 2017. 45:D362-368</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
@@ -465,7 +468,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -488,61 +491,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,6 +620,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -821,21 +891,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,711 +922,748 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="16">
         <v>40527</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="16">
         <v>42887</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="8" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="8" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="16">
         <v>42746</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="6" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="10" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="10" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="10" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="10" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="16">
         <v>41927</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="10" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="10" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="16">
         <v>40358</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="10" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="10" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="10" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="13" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="13" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="16">
         <v>42625</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="10" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="10" t="s">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="10" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="10" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="16">
         <v>42627</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="10" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="10">
         <v>42898</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="13" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="13" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E45" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="16">
         <v>42845</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="18" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="3"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="18" t="s">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="18" t="s">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="18" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="3"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="18" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="19">
         <v>42869</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="6" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="6" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="3"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="6" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="6" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="6" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="3"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="6" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="6" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="4" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A53:A60"/>
-    <mergeCell ref="B53:B60"/>
-    <mergeCell ref="C53:C60"/>
-    <mergeCell ref="D53:D60"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="D35:D39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="C40:C41"/>
@@ -1565,38 +1672,10 @@
     <mergeCell ref="B46:B51"/>
     <mergeCell ref="C46:C51"/>
     <mergeCell ref="D46:D51"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="C35:C39"/>
-    <mergeCell ref="D35:D39"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="D53:D61"/>
+    <mergeCell ref="C53:C61"/>
+    <mergeCell ref="B53:B61"/>
+    <mergeCell ref="A53:A61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>